<commit_message>
All persistence algorithm test done
</commit_message>
<xml_diff>
--- a/Laboratory1/src/data/TestDesign.xlsx
+++ b/Laboratory1/src/data/TestDesign.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MARIA ALEJANDRA\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Symghoul\Documents\AED\AEDLaboratory\Laboratory1\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{721E90BF-7289-4E9C-8F2F-E21A9B69329E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4695"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -50,12 +51,6 @@
     <t xml:space="preserve">Comprobar que el metodo cambia el estado a falso si el numero no es primo y true si así ocurre </t>
   </si>
   <si>
-    <t>Comprobar que el metodo agrega los numeros hasta el número que entra por parametro y no más</t>
-  </si>
-  <si>
-    <t>generarMatrix()</t>
-  </si>
-  <si>
     <t>verifyPrimePersistence()</t>
   </si>
   <si>
@@ -75,12 +70,18 @@
   </si>
   <si>
     <t xml:space="preserve">no tiene </t>
+  </si>
+  <si>
+    <t>generateMatrix()</t>
+  </si>
+  <si>
+    <t>Comprobar que el metodo agrega los numeros hasta el número que entra por parametro y ceros de ahí para alla</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -411,11 +412,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,22 +450,22 @@
     </row>
     <row r="2" spans="1:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>13</v>
-      </c>
       <c r="F2" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -475,16 +476,16 @@
         <v>6</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="E3" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>